<commit_message>
Included the reporting in ScriptingProvider file
</commit_message>
<xml_diff>
--- a/testdata/watson/xlsx/Book2.xlsx
+++ b/testdata/watson/xlsx/Book2.xlsx
@@ -70,52 +70,52 @@
     <t>I'll turn on the lights for you.</t>
   </si>
   <si>
+    <t>hi, what things can you do for me?</t>
+  </si>
+  <si>
+    <t>I'm trained to turn things on or off in the car dashboard, play music and find nearby amenities like restaurants, gas stations and restrooms.</t>
+  </si>
+  <si>
+    <t>ok, turn on the lights please</t>
+  </si>
+  <si>
+    <t>play some music</t>
+  </si>
+  <si>
+    <t>Sure thing! Which genre would you prefer? Jazz is my personal favorite.</t>
+  </si>
+  <si>
+    <t>My personal favorite is Rock</t>
+  </si>
+  <si>
+    <t>find near by restaurants for me</t>
+  </si>
+  <si>
+    <t>Of course. Do you have a specific cuisine in mind?</t>
+  </si>
+  <si>
+    <t>yes, Italian please</t>
+  </si>
+  <si>
+    <t>Super! I've found 5 locations for you. Which one would you like to drive to?</t>
+  </si>
+  <si>
+    <t>ok thank you, have a nice day</t>
+  </si>
+  <si>
+    <t>Okay! Speak to you soon.</t>
+  </si>
+  <si>
+    <t>Sure thing! The first restaurant gets great reviews.</t>
+  </si>
+  <si>
+    <t>To the nearest one, today at 8 pm</t>
+  </si>
+  <si>
+    <t>Ok, let's go to the restaurant at 8:00 PM, on Mon, 28 May 2018.</t>
+  </si>
+  <si>
     <t>Great choice! Playing some rock for you.</t>
-  </si>
-  <si>
-    <t>hi, what things can you do for me?</t>
-  </si>
-  <si>
-    <t>I'm trained to turn things on or off in the car dashboard, play music and find nearby amenities like restaurants, gas stations and restrooms.</t>
-  </si>
-  <si>
-    <t>ok, turn on the lights please</t>
-  </si>
-  <si>
-    <t>play some music</t>
-  </si>
-  <si>
-    <t>Sure thing! Which genre would you prefer? Jazz is my personal favorite.</t>
-  </si>
-  <si>
-    <t>My personal favorite is Rock</t>
-  </si>
-  <si>
-    <t>find near by restaurants for me</t>
-  </si>
-  <si>
-    <t>Of course. Do you have a specific cuisine in mind?</t>
-  </si>
-  <si>
-    <t>yes, Italian please</t>
-  </si>
-  <si>
-    <t>Super! I've found 5 locations for you. Which one would you like to drive to?</t>
-  </si>
-  <si>
-    <t>ok thank you, have a nice day</t>
-  </si>
-  <si>
-    <t>Okay! Speak to you soon.</t>
-  </si>
-  <si>
-    <t>Sure thing! The first restaurant gets great reviews.</t>
-  </si>
-  <si>
-    <t>To the nearest one, today at 8 pm</t>
-  </si>
-  <si>
-    <t>Ok, let's go to the restaurant at 8:00 PM, on Mon, 15 May 2018.</t>
   </si>
 </sst>
 </file>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,17 +516,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,67 +536,67 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +610,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes to point script to Watson Car bot
</commit_message>
<xml_diff>
--- a/testdata/watson/xlsx/Book2.xlsx
+++ b/testdata/watson/xlsx/Book2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33880\workspace\ChatBotAutomation\testdata\watson\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChatbotAPI\ChatBotAutomation\testdata\watson\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dialogs" sheetId="1" r:id="rId1"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>